<commit_message>
add sync.WG usage in zeropadding, im2col and flatten
</commit_message>
<xml_diff>
--- a/examples/simple_cnn/step_by_step_cnn(rgb dense inertia).xlsx
+++ b/examples/simple_cnn/step_by_step_cnn(rgb dense inertia).xlsx
@@ -648,8 +648,8 @@
   </sheetPr>
   <dimension ref="A1:AV107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD121" activeCellId="0" sqref="AD121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3162,7 +3162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="n">
         <f aca="false">A19+E19+I19</f>
         <v>28</v>
@@ -3176,7 +3176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="n">
         <f aca="false">A20+E20+I20</f>
         <v>23</v>
@@ -3190,7 +3190,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="17" t="s">
         <v>17</v>
       </c>
@@ -3215,7 +3216,7 @@
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="n">
         <f aca="false">A30+E30+I30</f>
         <v>9</v>

</xml_diff>

<commit_message>
fix excel: hidden rows
</commit_message>
<xml_diff>
--- a/examples/simple_cnn/step_by_step_cnn(rgb dense inertia).xlsx
+++ b/examples/simple_cnn/step_by_step_cnn(rgb dense inertia).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hp\go\src\github.com\LdDl\cnns\examples\simple_cnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C0EA36-8FBE-44D8-8E9B-7145EEBA84CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C436815-614B-41B9-ABEF-54268860D3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>5x5x3 Image representation</t>
   </si>
@@ -393,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,19 +429,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,35 +486,8 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:C43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -917,55 +920,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="41"/>
-      <c r="AE1" s="41"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="41"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
+      <c r="S1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
@@ -1594,66 +1597,66 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="O11" s="23" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="O11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
     </row>
     <row r="12" spans="1:48" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="E12" s="24" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="E12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="I12" s="24" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="I12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="S12" s="24" t="s">
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="S12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="W12" s="24" t="s">
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="W12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
@@ -1861,54 +1864,54 @@
       </c>
     </row>
     <row r="17" spans="1:42" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="I17" s="40" t="s">
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="I17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="23" t="s">
+      <c r="O17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="AB17" s="41" t="s">
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="AB17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="41"/>
-      <c r="AE17" s="41"/>
-      <c r="AF17" s="41"/>
-      <c r="AG17" s="41"/>
-      <c r="AH17" s="41"/>
-      <c r="AI17" s="41"/>
-      <c r="AJ17" s="41"/>
-      <c r="AK17" s="41"/>
-      <c r="AL17" s="41"/>
-      <c r="AM17" s="41"/>
-      <c r="AN17" s="41"/>
-      <c r="AO17" s="41"/>
-      <c r="AP17" s="41"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="24"/>
+      <c r="AI17" s="24"/>
+      <c r="AJ17" s="24"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="24"/>
+      <c r="AM17" s="24"/>
+      <c r="AN17" s="24"/>
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="24"/>
     </row>
     <row r="18" spans="1:42" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
@@ -2482,72 +2485,72 @@
       </c>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="23" t="s">
+      <c r="O23" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
     </row>
     <row r="24" spans="1:42" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="E24" s="24" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="E24" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="I24" s="24" t="s">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="I24" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="24" t="s">
+      <c r="O24" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="24" t="s">
+      <c r="S24" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="24" t="s">
+      <c r="W24" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
@@ -2772,52 +2775,52 @@
       <c r="Y28" s="11"/>
     </row>
     <row r="29" spans="1:42" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="I29" s="40" t="s">
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="I29" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="O29" s="23" t="s">
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="O29" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
-      <c r="AB29" s="41" t="s">
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="AB29" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AC29" s="41"/>
-      <c r="AD29" s="41"/>
-      <c r="AE29" s="41"/>
-      <c r="AF29" s="41"/>
-      <c r="AG29" s="41"/>
-      <c r="AH29" s="41"/>
-      <c r="AI29" s="41"/>
-      <c r="AJ29" s="41"/>
-      <c r="AK29" s="41"/>
-      <c r="AL29" s="41"/>
-      <c r="AM29" s="41"/>
-      <c r="AN29" s="41"/>
-      <c r="AO29" s="41"/>
-      <c r="AP29" s="41"/>
+      <c r="AC29" s="24"/>
+      <c r="AD29" s="24"/>
+      <c r="AE29" s="24"/>
+      <c r="AF29" s="24"/>
+      <c r="AG29" s="24"/>
+      <c r="AH29" s="24"/>
+      <c r="AI29" s="24"/>
+      <c r="AJ29" s="24"/>
+      <c r="AK29" s="24"/>
+      <c r="AL29" s="24"/>
+      <c r="AM29" s="24"/>
+      <c r="AN29" s="24"/>
+      <c r="AO29" s="24"/>
+      <c r="AP29" s="24"/>
     </row>
     <row r="30" spans="1:42" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
@@ -3364,13 +3367,13 @@
       </c>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-    </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+    </row>
+    <row r="36" spans="1:42" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <f>A18+E18+I18</f>
         <v>19</v>
@@ -3384,13 +3387,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
-        <f t="shared" ref="A36:C38" si="20">A19+E19+I19</f>
+        <f>A19+E19+I19</f>
         <v>28</v>
       </c>
       <c r="B37" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="A37:C38" si="20">B19+F19+J19</f>
         <v>16</v>
       </c>
       <c r="C37" s="13">
@@ -3398,9 +3401,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
-        <f t="shared" si="20"/>
+        <f>A20+E20+I20</f>
         <v>23</v>
       </c>
       <c r="B38" s="13">
@@ -3412,39 +3415,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:42" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34" t="s">
+    <row r="39" spans="1:42" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:42" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="F40" s="39" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="F40" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="O40" s="39" t="s">
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="O40" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="39"/>
-      <c r="R40" s="39"/>
-      <c r="S40" s="39"/>
-      <c r="T40" s="39"/>
-      <c r="U40" s="39"/>
-    </row>
-    <row r="41" spans="1:42" hidden="1" x14ac:dyDescent="0.2">
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+    </row>
+    <row r="41" spans="1:42" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
-        <f t="shared" ref="A41:C43" si="21">A30+E30+I30</f>
+        <f>A30+E30+I30</f>
         <v>9</v>
       </c>
       <c r="B41" s="13">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="B41:C41" si="21">B30+F30+J30</f>
         <v>1</v>
       </c>
       <c r="C41" s="13">
@@ -3468,16 +3471,16 @@
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
-        <f>A19+E19+I19</f>
-        <v>28</v>
+        <f>A31+E31+I31</f>
+        <v>-4</v>
       </c>
       <c r="B42" s="13">
-        <f t="shared" ref="B42:C42" si="22">B19+F19+J19</f>
-        <v>16</v>
+        <f t="shared" ref="B42:B43" si="22">B31+F31+J31</f>
+        <v>2</v>
       </c>
       <c r="C42" s="13">
-        <f t="shared" si="22"/>
-        <v>20</v>
+        <f t="shared" ref="C42:C43" si="23">C31+G31+K31</f>
+        <v>-2</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
@@ -3496,16 +3499,16 @@
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
-        <f>A20+E20+I20</f>
-        <v>23</v>
+        <f>A32+E32+I32</f>
+        <v>13</v>
       </c>
       <c r="B43" s="13">
-        <f t="shared" ref="B43:C43" si="23">B20+F20+J20</f>
-        <v>18</v>
+        <f t="shared" si="22"/>
+        <v>-4</v>
       </c>
       <c r="C43" s="13">
         <f t="shared" si="23"/>
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -3575,11 +3578,11 @@
       <c r="U44" s="14"/>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="14">
@@ -3615,11 +3618,11 @@
     </row>
     <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
-        <f t="shared" ref="A46:C48" si="26">IF(A36&gt;0,A36,0)</f>
+        <f>IF(A36&gt;0,A36,0)</f>
         <v>19</v>
       </c>
       <c r="B46" s="13">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="B46:C46" si="26">IF(B36&gt;0,B36,0)</f>
         <v>13</v>
       </c>
       <c r="C46" s="13">
@@ -3643,11 +3646,11 @@
     </row>
     <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
-        <f>IF(A42&gt;0,A42,0)</f>
+        <f t="shared" ref="A47:C47" si="27">IF(A37&gt;0,A37,0)</f>
         <v>28</v>
       </c>
       <c r="B47" s="13">
-        <f t="shared" ref="B47:C48" si="27">IF(B42&gt;0,B42,0)</f>
+        <f t="shared" si="27"/>
         <v>16</v>
       </c>
       <c r="C47" s="13">
@@ -3671,105 +3674,67 @@
     </row>
     <row r="48" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A48" s="13">
-        <f>IF(A43&gt;0,A43,0)</f>
+        <f t="shared" ref="A48:C48" si="28">IF(A38&gt;0,A38,0)</f>
         <v>23</v>
       </c>
       <c r="B48" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>18</v>
       </c>
       <c r="C48" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="E50" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
-        <f>IF(E51&gt;0,E51,0)</f>
+        <f>IF(A41&gt;0,A41,0)</f>
         <v>9</v>
       </c>
-      <c r="B51" s="15">
-        <f t="shared" ref="B51:C51" si="28">IF(F51&gt;0,F51,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C51" s="15">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="1">
-        <f>A30+E30+I30</f>
-        <v>9</v>
-      </c>
-      <c r="F51" s="1">
-        <f t="shared" ref="F51:G51" si="29">B30+F30+J30</f>
-        <v>1</v>
-      </c>
-      <c r="G51" s="1">
+      <c r="B51" s="23">
+        <f t="shared" ref="B51:C51" si="29">IF(B41&gt;0,B41,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C51" s="23">
         <f t="shared" si="29"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="15">
-        <f t="shared" ref="A52:A53" si="30">IF(E52&gt;0,E52,0)</f>
-        <v>0</v>
-      </c>
-      <c r="B52" s="15">
-        <f t="shared" ref="B52:B53" si="31">IF(F52&gt;0,F52,0)</f>
+      <c r="A52" s="23">
+        <f>IF(A42&gt;0,A42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B52" s="23">
+        <f t="shared" ref="A52:C52" si="30">IF(B42&gt;0,B42,0)</f>
         <v>2</v>
       </c>
-      <c r="C52" s="15">
-        <f t="shared" ref="C52:C53" si="32">IF(G52&gt;0,G52,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="1">
-        <f t="shared" ref="E52:E53" si="33">A31+E31+I31</f>
-        <v>-4</v>
-      </c>
-      <c r="F52" s="1">
-        <f t="shared" ref="F52:F53" si="34">B31+F31+J31</f>
-        <v>2</v>
-      </c>
-      <c r="G52" s="1">
-        <f t="shared" ref="G52:G53" si="35">C31+G31+K31</f>
-        <v>-2</v>
+      <c r="C52" s="23">
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="15">
-        <f t="shared" si="30"/>
+      <c r="A53" s="23">
+        <f>IF(A43&gt;0,A43,0)</f>
         <v>13</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="23">
+        <f t="shared" ref="A53:C53" si="31">IF(B43&gt;0,B43,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="23">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="C53" s="15">
-        <f t="shared" si="32"/>
-        <v>7</v>
-      </c>
-      <c r="E53" s="1">
-        <f t="shared" si="33"/>
-        <v>13</v>
-      </c>
-      <c r="F53" s="1">
-        <f t="shared" si="34"/>
-        <v>-4</v>
-      </c>
-      <c r="G53" s="1">
-        <f t="shared" si="35"/>
         <v>7</v>
       </c>
     </row>
@@ -3779,34 +3744,34 @@
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="N55" s="34" t="s">
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="N55" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O55" s="34"/>
-      <c r="P55" s="34"/>
+      <c r="O55" s="29"/>
+      <c r="P55" s="29"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
-      <c r="D56" s="37" t="s">
+      <c r="D56" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
       <c r="N56" s="14">
         <v>0</v>
       </c>
@@ -3850,16 +3815,16 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="N60" s="34" t="s">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="N60" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
+      <c r="O60" s="29"/>
+      <c r="P60" s="29"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="16">
@@ -3868,19 +3833,19 @@
       </c>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
-      <c r="D61" s="37" t="s">
+      <c r="D61" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E61" s="37" t="s">
+      <c r="E61" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="25"/>
+      <c r="L61" s="25"/>
       <c r="N61" s="17">
         <f>N81</f>
         <v>-1.4464257063467503E-3</v>
@@ -3921,27 +3886,27 @@
       </c>
     </row>
     <row r="66" spans="1:15" ht="46.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="F66" s="34" t="s">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="F66" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G66" s="34"/>
+      <c r="G66" s="29"/>
       <c r="I66" s="32" t="s">
         <v>30</v>
       </c>
       <c r="J66" s="32"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="26">
+      <c r="A67" s="33">
         <f>A57</f>
         <v>28</v>
       </c>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
       <c r="F67" s="7" t="s">
         <v>31</v>
       </c>
@@ -3956,12 +3921,12 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="26">
+      <c r="A68" s="33">
         <f>A61</f>
         <v>9</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
       <c r="F68" s="7" t="s">
         <v>33</v>
       </c>
@@ -4009,181 +3974,181 @@
     </row>
     <row r="73" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="E74" s="36" t="s">
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="E74" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="I74" s="25" t="s">
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
+      <c r="I74" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="J74" s="25"/>
-      <c r="K74" s="25"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="33">
+      <c r="A75" s="36">
         <f>F69*A67+G69*A68</f>
         <v>-5.4375542499999998</v>
       </c>
-      <c r="B75" s="33">
+      <c r="B75" s="36">
         <f>G69*B67+H69*B68</f>
         <v>0</v>
       </c>
-      <c r="C75" s="33">
+      <c r="C75" s="36">
         <f>H69*C67+I69*C68</f>
         <v>0</v>
       </c>
       <c r="D75" s="20"/>
-      <c r="E75" s="33">
+      <c r="E75" s="36">
         <f>TANH(A75)</f>
         <v>-0.99996215380996456</v>
       </c>
-      <c r="F75" s="33" t="e">
+      <c r="F75" s="36" t="e">
         <f>K69*F67+L69*F68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G75" s="33" t="e">
+      <c r="G75" s="36" t="e">
         <f>L69*G67+M69*G68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I75" s="33">
+      <c r="I75" s="36">
         <f>1-E75*E75</f>
         <v>7.5690947736739567E-5</v>
       </c>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A76" s="33">
+      <c r="A76" s="36">
         <f>F70*A67+G70*A68</f>
         <v>2.4813484900000007</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="E76" s="33">
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="E76" s="36">
         <f>TANH(A76)</f>
         <v>0.98610907450575491</v>
       </c>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="I76" s="33">
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="I76" s="36">
         <f>1-E76*E76</f>
         <v>2.758889317740354E-2</v>
       </c>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
+      <c r="J76" s="36"/>
+      <c r="K76" s="36"/>
     </row>
     <row r="79" spans="1:15" ht="58.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34" t="s">
+      <c r="A79" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B79" s="34"/>
-      <c r="D79" s="35" t="s">
+      <c r="B79" s="29"/>
+      <c r="D79" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E79" s="35"/>
-      <c r="G79" s="34" t="s">
+      <c r="E79" s="37"/>
+      <c r="G79" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H79" s="34"/>
+      <c r="H79" s="29"/>
       <c r="N79" s="32" t="s">
         <v>41</v>
       </c>
       <c r="O79" s="32"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A80" s="28">
+      <c r="A80" s="38">
         <v>0.15</v>
       </c>
-      <c r="B80" s="28"/>
-      <c r="D80" s="29">
+      <c r="B80" s="38"/>
+      <c r="D80" s="39">
         <f>E75-A80</f>
         <v>-1.1499621538099645</v>
       </c>
-      <c r="E80" s="29"/>
-      <c r="G80" s="30">
+      <c r="E80" s="39"/>
+      <c r="G80" s="40">
         <f>D80*I75</f>
         <v>-8.7041725283258482E-5</v>
       </c>
-      <c r="H80" s="30"/>
-      <c r="N80" s="31">
+      <c r="H80" s="40"/>
+      <c r="N80" s="41">
         <f>I69*G80+J69*G81</f>
         <v>9.3684703260546735E-4</v>
       </c>
-      <c r="O80" s="31"/>
+      <c r="O80" s="41"/>
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A81" s="28">
+      <c r="A81" s="38">
         <v>0.8</v>
       </c>
-      <c r="B81" s="28"/>
-      <c r="D81" s="29">
+      <c r="B81" s="38"/>
+      <c r="D81" s="39">
         <f>E76-A81</f>
         <v>0.18610907450575487</v>
       </c>
-      <c r="E81" s="29"/>
-      <c r="G81" s="30">
+      <c r="E81" s="39"/>
+      <c r="G81" s="40">
         <f>D81*I76</f>
         <v>5.1345433758847071E-3</v>
       </c>
-      <c r="H81" s="30"/>
-      <c r="N81" s="31">
+      <c r="H81" s="40"/>
+      <c r="N81" s="41">
         <f>I70*G80+J70*G81</f>
         <v>-1.4464257063467503E-3</v>
       </c>
-      <c r="O81" s="31"/>
+      <c r="O81" s="41"/>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="21">
         <v>0.01</v>
       </c>
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
       <c r="D86" s="21">
         <v>0.6</v>
       </c>
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="26"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="26"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="33"/>
     </row>
     <row r="90" spans="1:35" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="27" t="s">
+      <c r="A90" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B90" s="27"/>
-      <c r="E90" s="27" t="s">
+      <c r="B90" s="42"/>
+      <c r="E90" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F90" s="27"/>
-      <c r="H90" s="27" t="s">
+      <c r="F90" s="42"/>
+      <c r="H90" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="I90" s="27"/>
+      <c r="I90" s="42"/>
       <c r="AI90" s="1" t="s">
         <v>48</v>
       </c>
@@ -4277,92 +4242,92 @@
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A97" s="23" t="s">
+      <c r="A97" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
-      <c r="H97" s="23"/>
-      <c r="I97" s="23"/>
-      <c r="J97" s="23"/>
-      <c r="K97" s="23"/>
-      <c r="N97" s="23" t="s">
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="26"/>
+      <c r="K97" s="26"/>
+      <c r="N97" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="O97" s="23"/>
-      <c r="P97" s="23"/>
-      <c r="Q97" s="23"/>
-      <c r="R97" s="23"/>
-      <c r="S97" s="23"/>
-      <c r="T97" s="23"/>
-      <c r="U97" s="23"/>
-      <c r="V97" s="23"/>
-      <c r="W97" s="23"/>
-      <c r="X97" s="23"/>
-      <c r="Z97" s="23" t="s">
+      <c r="O97" s="26"/>
+      <c r="P97" s="26"/>
+      <c r="Q97" s="26"/>
+      <c r="R97" s="26"/>
+      <c r="S97" s="26"/>
+      <c r="T97" s="26"/>
+      <c r="U97" s="26"/>
+      <c r="V97" s="26"/>
+      <c r="W97" s="26"/>
+      <c r="X97" s="26"/>
+      <c r="Z97" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA97" s="23"/>
-      <c r="AB97" s="23"/>
-      <c r="AC97" s="23"/>
-      <c r="AD97" s="23"/>
-      <c r="AE97" s="23"/>
-      <c r="AF97" s="23"/>
-      <c r="AG97" s="23"/>
-      <c r="AH97" s="23"/>
-      <c r="AI97" s="23"/>
-      <c r="AJ97" s="23"/>
+      <c r="AA97" s="26"/>
+      <c r="AB97" s="26"/>
+      <c r="AC97" s="26"/>
+      <c r="AD97" s="26"/>
+      <c r="AE97" s="26"/>
+      <c r="AF97" s="26"/>
+      <c r="AG97" s="26"/>
+      <c r="AH97" s="26"/>
+      <c r="AI97" s="26"/>
+      <c r="AJ97" s="26"/>
     </row>
     <row r="98" spans="1:36" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A98" s="24" t="s">
+      <c r="A98" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="E98" s="24" t="s">
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="E98" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="I98" s="24" t="s">
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="I98" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J98" s="24"/>
-      <c r="K98" s="24"/>
-      <c r="N98" s="24" t="s">
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="N98" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="O98" s="24"/>
-      <c r="P98" s="24"/>
-      <c r="R98" s="24" t="s">
+      <c r="O98" s="27"/>
+      <c r="P98" s="27"/>
+      <c r="R98" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S98" s="24"/>
-      <c r="T98" s="24"/>
-      <c r="V98" s="24" t="s">
+      <c r="S98" s="27"/>
+      <c r="T98" s="27"/>
+      <c r="V98" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="W98" s="24"/>
-      <c r="X98" s="24"/>
-      <c r="Z98" s="24" t="s">
+      <c r="W98" s="27"/>
+      <c r="X98" s="27"/>
+      <c r="Z98" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AA98" s="24"/>
-      <c r="AB98" s="24"/>
-      <c r="AD98" s="24" t="s">
+      <c r="AA98" s="27"/>
+      <c r="AB98" s="27"/>
+      <c r="AD98" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AE98" s="24"/>
-      <c r="AF98" s="24"/>
-      <c r="AH98" s="24" t="s">
+      <c r="AE98" s="27"/>
+      <c r="AF98" s="27"/>
+      <c r="AH98" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AI98" s="24"/>
-      <c r="AJ98" s="24"/>
+      <c r="AI98" s="27"/>
+      <c r="AJ98" s="27"/>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
@@ -4394,370 +4359,370 @@
         <v>0</v>
       </c>
       <c r="N99" s="4">
-        <f t="shared" ref="N99:P101" si="36">(1-$D$86)*-1*$D$85*O18+$D$86*A99</f>
+        <f t="shared" ref="N99:P101" si="32">(1-$D$86)*-1*$D$85*O18+$D$86*A99</f>
         <v>-3.7473881304218697E-6</v>
       </c>
       <c r="O99" s="4">
+        <f t="shared" si="32"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="P99" s="4">
+        <f t="shared" si="32"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="R99" s="6">
+        <f t="shared" ref="R99:T101" si="33">(1-$D$86)*-1*$D$85*S18+$D$86*E99</f>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="S99" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="T99" s="6">
+        <f t="shared" si="33"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="V99" s="7">
+        <f t="shared" ref="V99:X101" si="34">(1-$D$86)*-1*$D$85*W18+$D$86*I99</f>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="W99" s="7">
+        <f t="shared" si="34"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="X99" s="7">
+        <f t="shared" si="34"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="Z99" s="4">
+        <f t="shared" ref="Z99:AB101" si="35">A13+N99</f>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="AA99" s="4">
+        <f t="shared" si="35"/>
+        <v>0.99999625261186953</v>
+      </c>
+      <c r="AB99" s="4">
+        <f t="shared" si="35"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="AD99" s="6">
+        <f t="shared" ref="AD99:AF101" si="36">E13+R99</f>
+        <v>1.9999925052237391</v>
+      </c>
+      <c r="AE99" s="6">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="AF99" s="6">
         <f t="shared" si="36"/>
         <v>-3.7473881304218697E-6</v>
       </c>
-      <c r="P99" s="4">
+      <c r="AH99" s="7">
+        <f t="shared" ref="AH99:AJ101" si="37">I13+V99</f>
+        <v>0.9999887578356087</v>
+      </c>
+      <c r="AI99" s="7">
+        <f t="shared" si="37"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="AJ99" s="7">
+        <f t="shared" si="37"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>0</v>
+      </c>
+      <c r="B100" s="4">
+        <v>0</v>
+      </c>
+      <c r="C100" s="4">
+        <v>0</v>
+      </c>
+      <c r="E100" s="6">
+        <v>0</v>
+      </c>
+      <c r="F100" s="6">
+        <f>B100</f>
+        <v>0</v>
+      </c>
+      <c r="G100" s="6">
+        <v>0</v>
+      </c>
+      <c r="I100" s="7">
+        <v>0</v>
+      </c>
+      <c r="J100" s="7">
+        <f>F100</f>
+        <v>0</v>
+      </c>
+      <c r="K100" s="7">
+        <v>0</v>
+      </c>
+      <c r="N100" s="4">
+        <f t="shared" si="32"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="O100" s="4">
+        <f t="shared" si="32"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="P100" s="4">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R100" s="6">
+        <f t="shared" si="33"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="S100" s="6">
+        <f t="shared" si="33"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="T100" s="6">
+        <f t="shared" si="33"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="V100" s="7">
+        <f t="shared" si="34"/>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="W100" s="7">
+        <f t="shared" si="34"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="X100" s="7">
+        <f t="shared" si="34"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="Z100" s="4">
+        <f t="shared" si="35"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="AA100" s="4">
+        <f t="shared" si="35"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="AB100" s="4">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="AD100" s="6">
         <f t="shared" si="36"/>
         <v>-1.124216439126561E-5</v>
       </c>
-      <c r="R99" s="6">
-        <f t="shared" ref="R99:T101" si="37">(1-$D$86)*-1*$D$85*S18+$D$86*E99</f>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="S99" s="6">
+      <c r="AE100" s="6">
+        <f t="shared" si="36"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="AF100" s="6">
+        <f t="shared" si="36"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+      <c r="AH100" s="7">
         <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="T99" s="6">
+        <v>0.99999250522373917</v>
+      </c>
+      <c r="AI100" s="7">
         <f t="shared" si="37"/>
         <v>-3.7473881304218697E-6</v>
       </c>
-      <c r="V99" s="7">
-        <f t="shared" ref="V99:X101" si="38">(1-$D$86)*-1*$D$85*W18+$D$86*I99</f>
+      <c r="AJ100" s="7">
+        <f t="shared" si="37"/>
+        <v>-3.7473881304218697E-6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A101" s="4">
+        <v>0</v>
+      </c>
+      <c r="B101" s="4">
+        <v>0</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+      <c r="E101" s="6">
+        <v>0</v>
+      </c>
+      <c r="F101" s="6">
+        <v>0</v>
+      </c>
+      <c r="G101" s="6">
+        <v>0</v>
+      </c>
+      <c r="I101" s="7">
+        <v>0</v>
+      </c>
+      <c r="J101" s="7">
+        <f>G100</f>
+        <v>0</v>
+      </c>
+      <c r="K101" s="7">
+        <v>0</v>
+      </c>
+      <c r="N101" s="4">
+        <f t="shared" si="32"/>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="O101" s="4">
+        <f t="shared" si="32"/>
         <v>-1.124216439126561E-5</v>
       </c>
-      <c r="W99" s="7">
-        <f t="shared" si="38"/>
+      <c r="P101" s="4">
+        <f t="shared" si="32"/>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="R101" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S101" s="6">
+        <f t="shared" si="33"/>
         <v>-1.124216439126561E-5</v>
       </c>
-      <c r="X99" s="7">
-        <f t="shared" si="38"/>
+      <c r="T101" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="V101" s="7">
+        <f t="shared" si="34"/>
+        <v>-1.124216439126561E-5</v>
+      </c>
+      <c r="W101" s="7">
+        <f t="shared" si="34"/>
         <v>-3.7473881304218697E-6</v>
       </c>
-      <c r="Z99" s="4">
-        <f t="shared" ref="Z99:AB101" si="39">A13+N99</f>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AA99" s="4">
-        <f t="shared" si="39"/>
-        <v>0.99999625261186953</v>
-      </c>
-      <c r="AB99" s="4">
-        <f t="shared" si="39"/>
+      <c r="X101" s="7">
+        <f t="shared" si="34"/>
         <v>-1.124216439126561E-5</v>
       </c>
-      <c r="AD99" s="6">
-        <f t="shared" ref="AD99:AF101" si="40">E13+R99</f>
-        <v>1.9999925052237391</v>
-      </c>
-      <c r="AE99" s="6">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-      <c r="AF99" s="6">
-        <f t="shared" si="40"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AH99" s="7">
-        <f t="shared" ref="AH99:AJ101" si="41">I13+V99</f>
+      <c r="Z101" s="4">
+        <f t="shared" si="35"/>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="AA101" s="4">
+        <f t="shared" si="35"/>
         <v>0.9999887578356087</v>
       </c>
-      <c r="AI99" s="7">
-        <f t="shared" si="41"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="AJ99" s="7">
-        <f t="shared" si="41"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A100" s="4">
-        <v>0</v>
-      </c>
-      <c r="B100" s="4">
-        <v>0</v>
-      </c>
-      <c r="C100" s="4">
-        <v>0</v>
-      </c>
-      <c r="E100" s="6">
-        <v>0</v>
-      </c>
-      <c r="F100" s="6">
-        <f>B100</f>
-        <v>0</v>
-      </c>
-      <c r="G100" s="6">
-        <v>0</v>
-      </c>
-      <c r="I100" s="7">
-        <v>0</v>
-      </c>
-      <c r="J100" s="7">
-        <f>F100</f>
-        <v>0</v>
-      </c>
-      <c r="K100" s="7">
-        <v>0</v>
-      </c>
-      <c r="N100" s="4">
+      <c r="AB101" s="4">
+        <f t="shared" si="35"/>
+        <v>-7.4947762608437393E-6</v>
+      </c>
+      <c r="AD101" s="6">
         <f t="shared" si="36"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="O100" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE101" s="6">
         <f t="shared" si="36"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="P100" s="4">
+        <v>2.9999887578356086</v>
+      </c>
+      <c r="AF101" s="6">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="R100" s="6">
+      <c r="AH101" s="7">
         <f t="shared" si="37"/>
         <v>-1.124216439126561E-5</v>
       </c>
-      <c r="S100" s="6">
+      <c r="AI101" s="7">
         <f t="shared" si="37"/>
         <v>-3.7473881304218697E-6</v>
       </c>
-      <c r="T100" s="6">
+      <c r="AJ101" s="7">
         <f t="shared" si="37"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="V100" s="7">
-        <f t="shared" si="38"/>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="W100" s="7">
-        <f t="shared" si="38"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="X100" s="7">
-        <f t="shared" si="38"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="Z100" s="4">
-        <f t="shared" si="39"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AA100" s="4">
-        <f t="shared" si="39"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AB100" s="4">
-        <f t="shared" si="39"/>
-        <v>2</v>
-      </c>
-      <c r="AD100" s="6">
-        <f t="shared" si="40"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="AE100" s="6">
-        <f t="shared" si="40"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AF100" s="6">
-        <f t="shared" si="40"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AH100" s="7">
-        <f t="shared" si="41"/>
-        <v>0.99999250522373917</v>
-      </c>
-      <c r="AI100" s="7">
-        <f t="shared" si="41"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AJ100" s="7">
-        <f t="shared" si="41"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A101" s="4">
-        <v>0</v>
-      </c>
-      <c r="B101" s="4">
-        <v>0</v>
-      </c>
-      <c r="C101" s="4">
-        <v>0</v>
-      </c>
-      <c r="E101" s="6">
-        <v>0</v>
-      </c>
-      <c r="F101" s="6">
-        <v>0</v>
-      </c>
-      <c r="G101" s="6">
-        <v>0</v>
-      </c>
-      <c r="I101" s="7">
-        <v>0</v>
-      </c>
-      <c r="J101" s="7">
-        <f>G100</f>
-        <v>0</v>
-      </c>
-      <c r="K101" s="7">
-        <v>0</v>
-      </c>
-      <c r="N101" s="4">
-        <f t="shared" si="36"/>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="O101" s="4">
-        <f t="shared" si="36"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="P101" s="4">
-        <f t="shared" si="36"/>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="R101" s="6">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="S101" s="6">
-        <f t="shared" si="37"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="T101" s="6">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="V101" s="7">
-        <f t="shared" si="38"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="W101" s="7">
-        <f t="shared" si="38"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="X101" s="7">
-        <f t="shared" si="38"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="Z101" s="4">
-        <f t="shared" si="39"/>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="AA101" s="4">
-        <f t="shared" si="39"/>
-        <v>0.9999887578356087</v>
-      </c>
-      <c r="AB101" s="4">
-        <f t="shared" si="39"/>
-        <v>-7.4947762608437393E-6</v>
-      </c>
-      <c r="AD101" s="6">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="AE101" s="6">
-        <f t="shared" si="40"/>
-        <v>2.9999887578356086</v>
-      </c>
-      <c r="AF101" s="6">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="AH101" s="7">
-        <f t="shared" si="41"/>
-        <v>-1.124216439126561E-5</v>
-      </c>
-      <c r="AI101" s="7">
-        <f t="shared" si="41"/>
-        <v>-3.7473881304218697E-6</v>
-      </c>
-      <c r="AJ101" s="7">
-        <f t="shared" si="41"/>
         <v>1.9999887578356088</v>
       </c>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B103" s="23"/>
-      <c r="C103" s="23"/>
-      <c r="D103" s="23"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="23"/>
-      <c r="H103" s="23"/>
-      <c r="I103" s="23"/>
-      <c r="J103" s="23"/>
-      <c r="K103" s="23"/>
-      <c r="N103" s="23" t="s">
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+      <c r="F103" s="26"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="26"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="26"/>
+      <c r="K103" s="26"/>
+      <c r="N103" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="O103" s="23"/>
-      <c r="P103" s="23"/>
-      <c r="Q103" s="23"/>
-      <c r="R103" s="23"/>
-      <c r="S103" s="23"/>
-      <c r="T103" s="23"/>
-      <c r="U103" s="23"/>
-      <c r="V103" s="23"/>
-      <c r="W103" s="23"/>
-      <c r="X103" s="23"/>
-      <c r="Z103" s="23" t="s">
+      <c r="O103" s="26"/>
+      <c r="P103" s="26"/>
+      <c r="Q103" s="26"/>
+      <c r="R103" s="26"/>
+      <c r="S103" s="26"/>
+      <c r="T103" s="26"/>
+      <c r="U103" s="26"/>
+      <c r="V103" s="26"/>
+      <c r="W103" s="26"/>
+      <c r="X103" s="26"/>
+      <c r="Z103" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="AA103" s="23"/>
-      <c r="AB103" s="23"/>
-      <c r="AC103" s="23"/>
-      <c r="AD103" s="23"/>
-      <c r="AE103" s="23"/>
-      <c r="AF103" s="23"/>
-      <c r="AG103" s="23"/>
-      <c r="AH103" s="23"/>
-      <c r="AI103" s="23"/>
-      <c r="AJ103" s="23"/>
+      <c r="AA103" s="26"/>
+      <c r="AB103" s="26"/>
+      <c r="AC103" s="26"/>
+      <c r="AD103" s="26"/>
+      <c r="AE103" s="26"/>
+      <c r="AF103" s="26"/>
+      <c r="AG103" s="26"/>
+      <c r="AH103" s="26"/>
+      <c r="AI103" s="26"/>
+      <c r="AJ103" s="26"/>
     </row>
     <row r="104" spans="1:36" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="E104" s="24" t="s">
+      <c r="B104" s="27"/>
+      <c r="C104" s="27"/>
+      <c r="E104" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="I104" s="24" t="s">
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="I104" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J104" s="24"/>
-      <c r="K104" s="24"/>
-      <c r="N104" s="24" t="s">
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="N104" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="O104" s="24"/>
-      <c r="P104" s="24"/>
-      <c r="R104" s="24" t="s">
+      <c r="O104" s="27"/>
+      <c r="P104" s="27"/>
+      <c r="R104" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S104" s="24"/>
-      <c r="T104" s="24"/>
-      <c r="V104" s="24" t="s">
+      <c r="S104" s="27"/>
+      <c r="T104" s="27"/>
+      <c r="V104" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="W104" s="24"/>
-      <c r="X104" s="24"/>
-      <c r="Z104" s="24" t="s">
+      <c r="W104" s="27"/>
+      <c r="X104" s="27"/>
+      <c r="Z104" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AA104" s="24"/>
-      <c r="AB104" s="24"/>
-      <c r="AD104" s="24" t="s">
+      <c r="AA104" s="27"/>
+      <c r="AB104" s="27"/>
+      <c r="AD104" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AE104" s="24"/>
-      <c r="AF104" s="24"/>
-      <c r="AH104" s="24" t="s">
+      <c r="AE104" s="27"/>
+      <c r="AF104" s="27"/>
+      <c r="AH104" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AI104" s="24"/>
-      <c r="AJ104" s="24"/>
+      <c r="AI104" s="27"/>
+      <c r="AJ104" s="27"/>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
@@ -4789,360 +4754,297 @@
         <v>0</v>
       </c>
       <c r="N105" s="4">
-        <f t="shared" ref="N105:P107" si="42">(1-$D$86)*-1*$D$85*O30+$D$86*A105</f>
+        <f t="shared" ref="N105:P107" si="38">(1-$D$86)*-1*$D$85*O30+$D$86*A105</f>
         <v>5.7857028253870016E-6</v>
       </c>
       <c r="O105" s="4">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="P105" s="4">
+        <f t="shared" si="38"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="R105" s="6">
+        <f t="shared" ref="R105:T107" si="39">(1-$D$86)*-1*$D$85*S30+$D$86*E105</f>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="S105" s="6">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="T105" s="6">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="V105" s="7">
+        <f t="shared" ref="V105:X107" si="40">(1-$D$86)*-1*$D$85*W30+$D$86*I105</f>
+        <v>1.1571405650774003E-5</v>
+      </c>
+      <c r="W105" s="7">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="X105" s="7">
+        <f t="shared" si="40"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="Z105" s="4">
+        <f t="shared" ref="Z105:AB107" si="41">A25+N105</f>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="AA105" s="4">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="AB105" s="4">
+        <f t="shared" si="41"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="AD105" s="6">
+        <f t="shared" ref="AD105:AF107" si="42">E25+R105</f>
+        <v>2.0000057857028253</v>
+      </c>
+      <c r="AE105" s="6">
         <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="P105" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF105" s="6">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AH105" s="7">
+        <f t="shared" ref="AH105:AJ107" si="43">I25+V105</f>
+        <v>1.0000115714056508</v>
+      </c>
+      <c r="AI105" s="7">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="7">
+        <f t="shared" si="43"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A106" s="4">
+        <v>0</v>
+      </c>
+      <c r="B106" s="4">
+        <v>0</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0</v>
+      </c>
+      <c r="E106" s="6">
+        <v>0</v>
+      </c>
+      <c r="F106" s="6">
+        <f>B106</f>
+        <v>0</v>
+      </c>
+      <c r="G106" s="6">
+        <v>0</v>
+      </c>
+      <c r="I106" s="7">
+        <v>0</v>
+      </c>
+      <c r="J106" s="7">
+        <f>F106</f>
+        <v>0</v>
+      </c>
+      <c r="K106" s="7">
+        <v>0</v>
+      </c>
+      <c r="N106" s="4">
+        <f t="shared" si="38"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="O106" s="4">
+        <f t="shared" si="38"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="P106" s="4">
+        <f t="shared" si="38"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="R106" s="6">
+        <f t="shared" si="39"/>
+        <v>1.1571405650774003E-5</v>
+      </c>
+      <c r="S106" s="6">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="T106" s="6">
+        <f t="shared" si="39"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="V106" s="7">
+        <f t="shared" si="40"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="W106" s="7">
+        <f t="shared" si="40"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="X106" s="7">
+        <f t="shared" si="40"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="Z106" s="4">
+        <f t="shared" si="41"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="AA106" s="4">
+        <f t="shared" si="41"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="AB106" s="4">
+        <f t="shared" si="41"/>
+        <v>2.0000173571084763</v>
+      </c>
+      <c r="AD106" s="6">
+        <f t="shared" si="42"/>
+        <v>1.1571405650774003E-5</v>
+      </c>
+      <c r="AE106" s="6">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AF106" s="6">
         <f t="shared" si="42"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="R105" s="6">
-        <f t="shared" ref="R105:T107" si="43">(1-$D$86)*-1*$D$85*S30+$D$86*E105</f>
+      <c r="AH106" s="7">
+        <f t="shared" si="43"/>
+        <v>1.0000173571084761</v>
+      </c>
+      <c r="AI106" s="7">
+        <f t="shared" si="43"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="AJ106" s="7">
+        <f t="shared" si="43"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="S105" s="6">
-        <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-      <c r="T105" s="6">
-        <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-      <c r="V105" s="7">
-        <f t="shared" ref="V105:X107" si="44">(1-$D$86)*-1*$D$85*W30+$D$86*I105</f>
+    </row>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A107" s="4">
+        <v>0</v>
+      </c>
+      <c r="B107" s="4">
+        <v>0</v>
+      </c>
+      <c r="C107" s="4">
+        <v>0</v>
+      </c>
+      <c r="E107" s="6">
+        <v>0</v>
+      </c>
+      <c r="F107" s="6">
+        <v>0</v>
+      </c>
+      <c r="G107" s="6">
+        <v>0</v>
+      </c>
+      <c r="I107" s="7">
+        <v>0</v>
+      </c>
+      <c r="J107" s="7">
+        <f>G106</f>
+        <v>0</v>
+      </c>
+      <c r="K107" s="7">
+        <v>0</v>
+      </c>
+      <c r="N107" s="4">
+        <f t="shared" si="38"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="O107" s="4">
+        <f t="shared" si="38"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="P107" s="4">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="R107" s="6">
+        <f t="shared" si="39"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="S107" s="6">
+        <f t="shared" si="39"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="T107" s="6">
+        <f t="shared" si="39"/>
+        <v>5.7857028253870016E-6</v>
+      </c>
+      <c r="V107" s="7">
+        <f t="shared" si="40"/>
         <v>1.1571405650774003E-5</v>
       </c>
-      <c r="W105" s="7">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="X105" s="7">
-        <f t="shared" si="44"/>
+      <c r="W107" s="7">
+        <f t="shared" si="40"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="Z105" s="4">
-        <f t="shared" ref="Z105:AB107" si="45">A25+N105</f>
+      <c r="X107" s="7">
+        <f t="shared" si="40"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="AA105" s="4">
-        <f t="shared" si="45"/>
-        <v>-1</v>
-      </c>
-      <c r="AB105" s="4">
-        <f t="shared" si="45"/>
+      <c r="Z107" s="4">
+        <f t="shared" si="41"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="AD105" s="6">
-        <f t="shared" ref="AD105:AF107" si="46">E25+R105</f>
-        <v>2.0000057857028253</v>
-      </c>
-      <c r="AE105" s="6">
-        <f t="shared" si="46"/>
-        <v>1</v>
-      </c>
-      <c r="AF105" s="6">
-        <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="AH105" s="7">
-        <f t="shared" ref="AH105:AJ107" si="47">I25+V105</f>
-        <v>1.0000115714056508</v>
-      </c>
-      <c r="AI105" s="7">
-        <f t="shared" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="AJ105" s="7">
-        <f t="shared" si="47"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A106" s="4">
-        <v>0</v>
-      </c>
-      <c r="B106" s="4">
-        <v>0</v>
-      </c>
-      <c r="C106" s="4">
-        <v>0</v>
-      </c>
-      <c r="E106" s="6">
-        <v>0</v>
-      </c>
-      <c r="F106" s="6">
-        <f>B106</f>
-        <v>0</v>
-      </c>
-      <c r="G106" s="6">
-        <v>0</v>
-      </c>
-      <c r="I106" s="7">
-        <v>0</v>
-      </c>
-      <c r="J106" s="7">
-        <f>F106</f>
-        <v>0</v>
-      </c>
-      <c r="K106" s="7">
-        <v>0</v>
-      </c>
-      <c r="N106" s="4">
+      <c r="AA107" s="4">
+        <f t="shared" si="41"/>
+        <v>1.0000057857028253</v>
+      </c>
+      <c r="AB107" s="4">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AD107" s="6">
+        <f t="shared" si="42"/>
+        <v>1.7357108476161003E-5</v>
+      </c>
+      <c r="AE107" s="6">
+        <f t="shared" si="42"/>
+        <v>-2.9999942142971747</v>
+      </c>
+      <c r="AF107" s="6">
         <f t="shared" si="42"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="O106" s="4">
-        <f t="shared" si="42"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="P106" s="4">
-        <f t="shared" si="42"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="R106" s="6">
+      <c r="AH107" s="7">
         <f t="shared" si="43"/>
         <v>1.1571405650774003E-5</v>
       </c>
-      <c r="S106" s="6">
-        <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-      <c r="T106" s="6">
+      <c r="AI107" s="7">
         <f t="shared" si="43"/>
         <v>5.7857028253870016E-6</v>
       </c>
-      <c r="V106" s="7">
-        <f t="shared" si="44"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="W106" s="7">
-        <f t="shared" si="44"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="X106" s="7">
-        <f t="shared" si="44"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="Z106" s="4">
-        <f t="shared" si="45"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AA106" s="4">
-        <f t="shared" si="45"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AB106" s="4">
-        <f t="shared" si="45"/>
-        <v>2.0000173571084763</v>
-      </c>
-      <c r="AD106" s="6">
-        <f t="shared" si="46"/>
-        <v>1.1571405650774003E-5</v>
-      </c>
-      <c r="AE106" s="6">
-        <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="AF106" s="6">
-        <f t="shared" si="46"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AH106" s="7">
-        <f t="shared" si="47"/>
-        <v>1.0000173571084761</v>
-      </c>
-      <c r="AI106" s="7">
-        <f t="shared" si="47"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="AJ106" s="7">
-        <f t="shared" si="47"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A107" s="4">
-        <v>0</v>
-      </c>
-      <c r="B107" s="4">
-        <v>0</v>
-      </c>
-      <c r="C107" s="4">
-        <v>0</v>
-      </c>
-      <c r="E107" s="6">
-        <v>0</v>
-      </c>
-      <c r="F107" s="6">
-        <v>0</v>
-      </c>
-      <c r="G107" s="6">
-        <v>0</v>
-      </c>
-      <c r="I107" s="7">
-        <v>0</v>
-      </c>
-      <c r="J107" s="7">
-        <f>G106</f>
-        <v>0</v>
-      </c>
-      <c r="K107" s="7">
-        <v>0</v>
-      </c>
-      <c r="N107" s="4">
-        <f t="shared" si="42"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="O107" s="4">
-        <f t="shared" si="42"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="P107" s="4">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="R107" s="6">
+      <c r="AJ107" s="7">
         <f t="shared" si="43"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="S107" s="6">
-        <f t="shared" si="43"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="T107" s="6">
-        <f t="shared" si="43"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="V107" s="7">
-        <f t="shared" si="44"/>
-        <v>1.1571405650774003E-5</v>
-      </c>
-      <c r="W107" s="7">
-        <f t="shared" si="44"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="X107" s="7">
-        <f t="shared" si="44"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="Z107" s="4">
-        <f t="shared" si="45"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AA107" s="4">
-        <f t="shared" si="45"/>
-        <v>1.0000057857028253</v>
-      </c>
-      <c r="AB107" s="4">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AD107" s="6">
-        <f t="shared" si="46"/>
-        <v>1.7357108476161003E-5</v>
-      </c>
-      <c r="AE107" s="6">
-        <f t="shared" si="46"/>
-        <v>-2.9999942142971747</v>
-      </c>
-      <c r="AF107" s="6">
-        <f t="shared" si="46"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AH107" s="7">
-        <f t="shared" si="47"/>
-        <v>1.1571405650774003E-5</v>
-      </c>
-      <c r="AI107" s="7">
-        <f t="shared" si="47"/>
-        <v>5.7857028253870016E-6</v>
-      </c>
-      <c r="AJ107" s="7">
-        <f t="shared" si="47"/>
         <v>-1.9999942142971747</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="S1:AG1"/>
-    <mergeCell ref="AI1:AN1"/>
-    <mergeCell ref="AQ1:AV1"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="O11:Y11"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="O17:Y17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="AB17:AP17"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="O23:Y23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="O29:Y29"/>
-    <mergeCell ref="AB29:AP29"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="F40:L40"/>
-    <mergeCell ref="O40:U40"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="D56:L56"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="D61:L61"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="I75:K75"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="I76:K76"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="N79:O79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A88:I88"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="A103:K103"/>
+    <mergeCell ref="N103:X103"/>
+    <mergeCell ref="Z103:AJ103"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="E104:G104"/>
+    <mergeCell ref="I104:K104"/>
+    <mergeCell ref="N104:P104"/>
+    <mergeCell ref="R104:T104"/>
+    <mergeCell ref="V104:X104"/>
+    <mergeCell ref="Z104:AB104"/>
+    <mergeCell ref="AD104:AF104"/>
+    <mergeCell ref="AH104:AJ104"/>
     <mergeCell ref="A97:K97"/>
     <mergeCell ref="N97:X97"/>
     <mergeCell ref="Z97:AJ97"/>
@@ -5155,18 +5057,81 @@
     <mergeCell ref="Z98:AB98"/>
     <mergeCell ref="AD98:AF98"/>
     <mergeCell ref="AH98:AJ98"/>
-    <mergeCell ref="A103:K103"/>
-    <mergeCell ref="N103:X103"/>
-    <mergeCell ref="Z103:AJ103"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="E104:G104"/>
-    <mergeCell ref="I104:K104"/>
-    <mergeCell ref="N104:P104"/>
-    <mergeCell ref="R104:T104"/>
-    <mergeCell ref="V104:X104"/>
-    <mergeCell ref="Z104:AB104"/>
-    <mergeCell ref="AD104:AF104"/>
-    <mergeCell ref="AH104:AJ104"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A88:I88"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="N79:O79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="I76:K76"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="I75:K75"/>
+    <mergeCell ref="D61:L61"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="D56:L56"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="F40:L40"/>
+    <mergeCell ref="O40:U40"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="O29:Y29"/>
+    <mergeCell ref="AB29:AP29"/>
+    <mergeCell ref="AB17:AP17"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="O23:Y23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="O17:Y17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="S1:AG1"/>
+    <mergeCell ref="AI1:AN1"/>
+    <mergeCell ref="AQ1:AV1"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="O11:Y11"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>